<commit_message>
plot work for CIE review
</commit_message>
<xml_diff>
--- a/Production_models/Output/Sims/sim_results_summary.xlsx
+++ b/Production_models/Output/Sims/sim_results_summary.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjjoy\Documents\Groundfish Biometrics\Yelloweye_Production_Models\YE_Production_SEO\Model Output\PHASE3_B1-1_B2-1_upv-5_phmu-0.7_phsig-1.2_Kmu-10.6_Ksig-9.2_derb_0_1500k\simulations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjjoy\Documents\Groundfish Biometrics\SEO_DSR\seak_seo_dsr\Production_models\Output\Sims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{75479FE9-FF3B-479F-A982-DB2AC7A06A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84D45BE-E9E7-487F-B819-D48CC738F4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37200" yWindow="1665" windowWidth="15060" windowHeight="13530"/>
+    <workbookView xWindow="30180" yWindow="885" windowWidth="21600" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sim_results_summary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="40">
   <si>
     <t>parameter</t>
   </si>
@@ -74,16 +87,135 @@
   </si>
   <si>
     <t>sigma</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>EYKT</t>
+  </si>
+  <si>
+    <t>NSEO</t>
+  </si>
+  <si>
+    <t>CSEO</t>
+  </si>
+  <si>
+    <t>SSEO</t>
+  </si>
+  <si>
+    <t>true r</t>
+  </si>
+  <si>
+    <t>mean sim r</t>
+  </si>
+  <si>
+    <t>mean bias</t>
+  </si>
+  <si>
+    <t>true K</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">true </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <t>mean sim K</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mean sim </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <t>95% CI dontains true X% of time</t>
+  </si>
+  <si>
+    <t>true pi</t>
+  </si>
+  <si>
+    <t>mean sim pi</t>
+  </si>
+  <si>
+    <t>mean sim</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>B</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>I</t>
+    </r>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>mngmt area</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +350,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -400,7 +569,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -515,6 +684,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -560,9 +747,103 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -917,16 +1198,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -955,7 +1246,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -987,7 +1278,7 @@
         <v>-0.60875000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1019,7 +1310,7 @@
         <v>-0.58608695652173903</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1050,8 +1341,39 @@
       <c r="J4" s="1">
         <v>-0.64533333333333298</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M4" s="2"/>
+      <c r="N4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="V4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="W4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="X4" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1082,12 +1404,76 @@
       <c r="J5" s="1">
         <v>-0.68307692307692303</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="O5" s="14">
+        <v>9.6600000000000002E-3</v>
+      </c>
+      <c r="P5" s="1">
+        <v>-0.39624999999999999</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>0.94</v>
+      </c>
+      <c r="S5" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" s="4">
+        <v>1.6E-2</v>
+      </c>
+      <c r="V5" s="27">
+        <v>9.6600000000000002E-3</v>
+      </c>
+      <c r="W5" s="28">
+        <v>-0.39624999999999999</v>
+      </c>
+      <c r="X5" s="29">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="7">
+        <v>2.3E-2</v>
+      </c>
+      <c r="O6" s="14">
+        <v>1.447E-2</v>
+      </c>
+      <c r="P6" s="1">
+        <v>-0.37086956521739101</v>
+      </c>
+      <c r="Q6" s="15">
+        <v>0.93</v>
+      </c>
+      <c r="S6" s="30"/>
+      <c r="T6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6" s="6">
+        <v>2.3E-2</v>
+      </c>
+      <c r="V6" s="27">
+        <v>1.447E-2</v>
+      </c>
+      <c r="W6" s="28">
+        <v>-0.37086956521739101</v>
+      </c>
+      <c r="X6" s="29">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1118,8 +1504,39 @@
       <c r="J7" s="1">
         <v>-0.17049729901079699</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O7" s="14">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="P7" s="1">
+        <v>-0.51333333333333298</v>
+      </c>
+      <c r="Q7" s="15">
+        <v>0.77</v>
+      </c>
+      <c r="S7" s="30"/>
+      <c r="T7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="U7" s="6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="V7" s="27">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="W7" s="28">
+        <v>-0.51333333333333298</v>
+      </c>
+      <c r="X7" s="29">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1150,8 +1567,39 @@
       <c r="J8" s="1">
         <v>-2.49837204230011E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="9">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="O8" s="19">
+        <v>6.8700000000000002E-3</v>
+      </c>
+      <c r="P8" s="20">
+        <v>-0.47153846153846202</v>
+      </c>
+      <c r="Q8" s="21">
+        <v>0.87</v>
+      </c>
+      <c r="S8" s="31"/>
+      <c r="T8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="U8" s="8">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="V8" s="32">
+        <v>6.8700000000000002E-3</v>
+      </c>
+      <c r="W8" s="33">
+        <v>-0.47153846153846202</v>
+      </c>
+      <c r="X8" s="34">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1182,8 +1630,26 @@
       <c r="J9" s="1">
         <v>-0.139327866527373</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="S9" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U9" s="35">
+        <v>10091.7655000004</v>
+      </c>
+      <c r="V9" s="35">
+        <v>9851.6888600000002</v>
+      </c>
+      <c r="W9" s="28">
+        <v>-2.3789359750818698E-2</v>
+      </c>
+      <c r="X9" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1214,12 +1680,57 @@
       <c r="J10" s="1">
         <v>-0.199416249592612</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="S10" s="30"/>
+      <c r="T10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="U10" s="35">
+        <v>4642.21213000019</v>
+      </c>
+      <c r="V10" s="35">
+        <v>6072.7457599999998</v>
+      </c>
+      <c r="W10" s="28">
+        <v>0.30815774676797297</v>
+      </c>
+      <c r="X10" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M11" s="2"/>
+      <c r="N11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q11" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="S11" s="30"/>
+      <c r="T11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="U11" s="35">
+        <v>14047.7375760006</v>
+      </c>
+      <c r="V11" s="35">
+        <v>13578.590759999999</v>
+      </c>
+      <c r="W11" s="28">
+        <v>-3.3396610198788999E-2</v>
+      </c>
+      <c r="X11" s="29">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1250,8 +1761,39 @@
       <c r="J12" s="1">
         <v>-0.60717338812643395</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12">
+        <v>10091.7655000004</v>
+      </c>
+      <c r="O12">
+        <v>9851.6888600000002</v>
+      </c>
+      <c r="P12" s="1">
+        <v>-2.3789359750818698E-2</v>
+      </c>
+      <c r="Q12" s="15">
+        <v>1</v>
+      </c>
+      <c r="S12" s="31"/>
+      <c r="T12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="U12" s="36">
+        <v>11625.713856000501</v>
+      </c>
+      <c r="V12" s="36">
+        <v>10783.69253</v>
+      </c>
+      <c r="W12" s="33">
+        <v>-7.2427494468726497E-2</v>
+      </c>
+      <c r="X12" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1282,8 +1824,41 @@
       <c r="J13" s="1">
         <v>-0.58518646261596297</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13">
+        <v>4642.21213000019</v>
+      </c>
+      <c r="O13">
+        <v>6072.7457599999998</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0.30815774676797297</v>
+      </c>
+      <c r="Q13" s="15">
+        <v>1</v>
+      </c>
+      <c r="S13" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U13" s="6">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="V13" s="6">
+        <v>0.67098999999999998</v>
+      </c>
+      <c r="W13" s="28">
+        <v>-0.12174083769633499</v>
+      </c>
+      <c r="X13" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1314,8 +1889,39 @@
       <c r="J14" s="1">
         <v>-0.64197579621050704</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14">
+        <v>14047.7375760006</v>
+      </c>
+      <c r="O14">
+        <v>13578.590759999999</v>
+      </c>
+      <c r="P14" s="1">
+        <v>-3.3396610198788999E-2</v>
+      </c>
+      <c r="Q14" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="S14" s="30"/>
+      <c r="T14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="U14" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="V14" s="6">
+        <v>0.55173000000000005</v>
+      </c>
+      <c r="W14" s="28">
+        <v>3.1454545454545602E-3</v>
+      </c>
+      <c r="X14" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1346,12 +1952,60 @@
       <c r="J15" s="1">
         <v>-0.682859771830444</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15">
+        <v>11625.713856000501</v>
+      </c>
+      <c r="O15">
+        <v>10783.69253</v>
+      </c>
+      <c r="P15" s="1">
+        <v>-7.2427494468726497E-2</v>
+      </c>
+      <c r="Q15" s="15">
+        <v>1</v>
+      </c>
+      <c r="S15" s="30"/>
+      <c r="T15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="U15" s="6">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="V15" s="6">
+        <v>0.73814999999999997</v>
+      </c>
+      <c r="W15" s="28">
+        <v>-0.109589867310012</v>
+      </c>
+      <c r="X15" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="Q16" s="15"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="U16" s="8">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="V16" s="8">
+        <v>0.70618000000000003</v>
+      </c>
+      <c r="W16" s="33">
+        <v>-0.13032019704433501</v>
+      </c>
+      <c r="X16" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1382,8 +2036,39 @@
       <c r="J17" s="1">
         <v>-0.17049729058808799</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M17" s="2"/>
+      <c r="N17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q17" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="S17" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U17" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="V17" s="6">
+        <v>0.24468999999999999</v>
+      </c>
+      <c r="W17" s="28">
+        <v>-2.1239999999999998E-2</v>
+      </c>
+      <c r="X17" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1414,8 +2099,39 @@
       <c r="J18" s="1">
         <v>-2.4983704266910399E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N18">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="O18">
+        <v>0.67098999999999998</v>
+      </c>
+      <c r="P18" s="1">
+        <v>-0.12174083769633499</v>
+      </c>
+      <c r="Q18" s="15">
+        <v>1</v>
+      </c>
+      <c r="S18" s="30"/>
+      <c r="T18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="U18" s="6">
+        <v>0.115</v>
+      </c>
+      <c r="V18" s="6">
+        <v>0.14882999999999999</v>
+      </c>
+      <c r="W18" s="28">
+        <v>0.29417391304347801</v>
+      </c>
+      <c r="X18" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1446,8 +2162,39 @@
       <c r="J19" s="1">
         <v>-0.13932787151038201</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N19">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O19">
+        <v>0.55173000000000005</v>
+      </c>
+      <c r="P19" s="1">
+        <v>3.1454545454545602E-3</v>
+      </c>
+      <c r="Q19" s="15">
+        <v>1</v>
+      </c>
+      <c r="S19" s="30"/>
+      <c r="T19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="U19" s="6">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="V19" s="6">
+        <v>0.33877000000000002</v>
+      </c>
+      <c r="W19" s="28">
+        <v>-2.6522988505747001E-2</v>
+      </c>
+      <c r="X19" s="29">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1478,12 +2225,76 @@
       <c r="J20" s="1">
         <v>-0.199416249592612</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="O20">
+        <v>0.73814999999999997</v>
+      </c>
+      <c r="P20" s="1">
+        <v>-0.109589867310012</v>
+      </c>
+      <c r="Q20" s="15">
+        <v>1</v>
+      </c>
+      <c r="S20" s="31"/>
+      <c r="T20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="U20" s="8">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="V20" s="8">
+        <v>0.26768999999999998</v>
+      </c>
+      <c r="W20" s="33">
+        <v>-7.0520833333333297E-2</v>
+      </c>
+      <c r="X20" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="O21">
+        <v>0.70618000000000003</v>
+      </c>
+      <c r="P21" s="1">
+        <v>-0.13032019704433501</v>
+      </c>
+      <c r="Q21" s="15">
+        <v>1</v>
+      </c>
+      <c r="S21" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="T21" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="U21" s="6">
+        <v>0.373</v>
+      </c>
+      <c r="V21" s="6">
+        <v>0.41659000000000002</v>
+      </c>
+      <c r="W21" s="28">
+        <v>0.11686327077748</v>
+      </c>
+      <c r="X21" s="29">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>17</v>
       </c>
@@ -1514,8 +2325,27 @@
       <c r="J22" s="1">
         <v>-0.64773231540110998</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="Q22" s="15"/>
+      <c r="S22" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="T22" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="U22" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V22" s="6">
+        <v>0.14529</v>
+      </c>
+      <c r="W22" s="28">
+        <v>3.77857142857142E-2</v>
+      </c>
+      <c r="X22" s="29">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>18</v>
       </c>
@@ -1546,8 +2376,39 @@
       <c r="J23" s="1">
         <v>-0.55843463431859897</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M23" s="2"/>
+      <c r="N23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="P23" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q23" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="S23" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="T23" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="U23" s="8">
+        <v>0.23664319132398401</v>
+      </c>
+      <c r="V23" s="8">
+        <v>4.6120000000000001E-2</v>
+      </c>
+      <c r="W23" s="33">
+        <v>-0.80510742885960396</v>
+      </c>
+      <c r="X23" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>19</v>
       </c>
@@ -1578,8 +2439,23 @@
       <c r="J24" s="1">
         <v>-0.67984148365651798</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N24">
+        <v>0.25</v>
+      </c>
+      <c r="O24">
+        <v>0.24468999999999999</v>
+      </c>
+      <c r="P24" s="1">
+        <v>-2.1239999999999998E-2</v>
+      </c>
+      <c r="Q24" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20</v>
       </c>
@@ -1610,12 +2486,42 @@
       <c r="J25" s="1">
         <v>-0.73068428268294505</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N25">
+        <v>0.115</v>
+      </c>
+      <c r="O25">
+        <v>0.14882999999999999</v>
+      </c>
+      <c r="P25" s="1">
+        <v>0.29417391304347801</v>
+      </c>
+      <c r="Q25" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N26">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="O26">
+        <v>0.33877000000000002</v>
+      </c>
+      <c r="P26" s="1">
+        <v>-2.6522988505747001E-2</v>
+      </c>
+      <c r="Q26" s="15">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>21</v>
       </c>
@@ -1646,8 +2552,23 @@
       <c r="J27" s="1">
         <v>-0.126217277486911</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="O27">
+        <v>0.26768999999999998</v>
+      </c>
+      <c r="P27" s="1">
+        <v>-7.0520833333333297E-2</v>
+      </c>
+      <c r="Q27" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>22</v>
       </c>
@@ -1678,8 +2599,9 @@
       <c r="J28" s="1">
         <v>-5.7145454545454701E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="Q28" s="15"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>23</v>
       </c>
@@ -1710,8 +2632,21 @@
       <c r="J29" s="1">
         <v>-0.10159227985524701</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M29" s="2"/>
+      <c r="N29" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O29" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="P29" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q29" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>24</v>
       </c>
@@ -1742,12 +2677,42 @@
       <c r="J30" s="1">
         <v>-0.12538177339901499</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M30" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="N30">
+        <v>0.373</v>
+      </c>
+      <c r="O30">
+        <v>0.41659000000000002</v>
+      </c>
+      <c r="P30" s="1">
+        <v>0.11686327077748</v>
+      </c>
+      <c r="Q30" s="15">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M31" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="N31">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O31">
+        <v>0.14529</v>
+      </c>
+      <c r="P31" s="1">
+        <v>3.77857142857142E-2</v>
+      </c>
+      <c r="Q31" s="15">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>25</v>
       </c>
@@ -1778,8 +2743,23 @@
       <c r="J32" s="1">
         <v>-0.11391999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M32" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="N32" s="23">
+        <v>0.23664319132398401</v>
+      </c>
+      <c r="O32" s="23">
+        <v>4.6120000000000001E-2</v>
+      </c>
+      <c r="P32" s="20">
+        <v>-0.80510742885960396</v>
+      </c>
+      <c r="Q32" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>26</v>
       </c>
@@ -1810,8 +2790,12 @@
       <c r="J33" s="1">
         <v>3.2000000000000001E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M33" s="8"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="9"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>27</v>
       </c>
@@ -1843,7 +2827,7 @@
         <v>-7.52011494252873E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>28</v>
       </c>
@@ -1875,11 +2859,11 @@
         <v>-0.14447916666666699</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>29</v>
       </c>
@@ -1911,11 +2895,11 @@
         <v>6.4959785522788305E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>30</v>
       </c>
@@ -1947,11 +2931,11 @@
         <v>3.2642857142857098E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>31</v>
       </c>
@@ -1983,9 +2967,53 @@
         <v>-0.80861481901672705</v>
       </c>
     </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <f>C41^2</f>
+        <v>5.5999999999999703E-2</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>4.6120000000000001E-2</v>
+      </c>
+      <c r="F43">
+        <v>4.5289999999999997E-2</v>
+      </c>
+      <c r="G43">
+        <v>-0.19052319132398399</v>
+      </c>
+      <c r="H43">
+        <v>-0.19135319132398401</v>
+      </c>
+      <c r="I43" s="1">
+        <f>(C43-E43)/C43</f>
+        <v>0.17642857142856702</v>
+      </c>
+      <c r="J43" s="1">
+        <v>-0.80861481901672705</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="S5:S8"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="S13:S16"/>
+    <mergeCell ref="S17:S20"/>
+  </mergeCells>
   <conditionalFormatting sqref="D2:D39">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D41">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1995,7 +3023,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J39">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2006,7 +3034,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D41">
+  <conditionalFormatting sqref="I2:J41">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2016,7 +3056,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:J41">
+  <conditionalFormatting sqref="I43:J43">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>